<commit_message>
after fix and more new func
</commit_message>
<xml_diff>
--- a/temp/export/export_data.xlsx
+++ b/temp/export/export_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,62 +424,285 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>serial number</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>serial number</t>
+          <t>activated date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>activated date</t>
+          <t>pay_day</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>pay_day</t>
+          <t>pre-pay day</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>pre-pay day</t>
+          <t>on pause</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>on pause</t>
+          <t>phone</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>telegram username</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>telegram username</t>
+          <t>username</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>username</t>
+          <t>email</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>password</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>password</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
           <t>pay_list</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>KIT400848944</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>11/18/2024</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>+7 959 502 9416</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>@M98_FaZa</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Фаза</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>84@zov.icu</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Password1236</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>341525</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>KIT400864544</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11/18/2024</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>+7 904 902 4696</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>@tankist613</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Alex210949 Alex210949</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>84@zov.icu</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Password1237</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>341526</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>KIT400594583</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>11/18/2024</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>+nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Илья .</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>84@zov.icu</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Password1238</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>341527</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>KIT400594582131234</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>11/18/2024</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>11/19/2024</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>11/20/2024</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>+32142134213</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>asdsa</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Илья .</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>84@zov.icu</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Password1238</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>341527</t>
         </is>
       </c>
     </row>

</xml_diff>